<commit_message>
modified some viz for better readability
</commit_message>
<xml_diff>
--- a/data/feature_description.xlsx
+++ b/data/feature_description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cynthiax/Desktop/DATA1030/data1030-load-default-prob/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cynthiax/Desktop/DATA1030/data1030-loan-default-prob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CFE2B-10DF-1B4A-8116-81FF3AB82D5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53927FA-63A5-1344-8138-B4D9BEA0BF44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11260" yWindow="1060" windowWidth="17540" windowHeight="15080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14020" yWindow="500" windowWidth="17540" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStatsFull" sheetId="2" r:id="rId1"/>
@@ -1366,7 +1366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5DE156-7394-1F48-AEFB-7481540F7501}">
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1501,305 +1503,305 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>108</v>
+    <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>109</v>
+        <v>293</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>111</v>
+    <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>114</v>
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>116</v>
+    <row r="21" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>117</v>
+        <v>16</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>21</v>
+      <c r="A24" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>120</v>
+        <v>18</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>122</v>
+      <c r="A27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>123</v>
+      <c r="A28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C29" s="10"/>
     </row>
-    <row r="30" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>126</v>
+    <row r="30" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>128</v>
+        <v>271</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>129</v>
+        <v>272</v>
       </c>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>130</v>
+        <v>281</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>131</v>
+        <v>282</v>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>132</v>
+    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>133</v>
+    <row r="35" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>134</v>
+    <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>135</v>
+    <row r="37" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="C37" s="4"/>
       <c r="I37" s="11"/>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="1:11" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>136</v>
+    <row r="38" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>137</v>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>138</v>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>139</v>
+      <c r="A41" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>140</v>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>268</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>141</v>
+      <c r="A43" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>143</v>
+        <v>26</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>145</v>
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>147</v>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="D46" s="5"/>
       <c r="I46" s="11"/>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>148</v>
+    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="D47" s="5"/>
       <c r="I47" s="11"/>
@@ -1808,10 +1810,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>149</v>
+        <v>128</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="D48" s="5"/>
       <c r="I48" s="13"/>
@@ -1820,617 +1822,617 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>150</v>
+        <v>130</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>151</v>
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>152</v>
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>154</v>
+        <v>31</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>156</v>
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>160</v>
+    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>161</v>
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>163</v>
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>164</v>
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>166</v>
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="D59" s="5"/>
     </row>
     <row r="60" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>168</v>
+        <v>142</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="D60" s="5"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>169</v>
+        <v>144</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>170</v>
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>176</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>178</v>
+      <c r="A69" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>179</v>
+        <v>159</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>58</v>
+      <c r="A73" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="C73"/>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>185</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>187</v>
+        <v>46</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>189</v>
+        <v>47</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>191</v>
+        <v>48</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>193</v>
+        <v>49</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>197</v>
+        <v>50</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>201</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>204</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>208</v>
+      <c r="A91" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>211</v>
+        <v>188</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>77</v>
+        <v>285</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>215</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>221</v>
+        <v>64</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A104" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>224</v>
+        <v>69</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="6" t="s">
-        <v>86</v>
+      <c r="A109" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>232</v>
+        <v>71</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>234</v>
+      <c r="A115" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -2442,227 +2444,227 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="B125" s="15" t="s">
-        <v>253</v>
+      <c r="A125" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>255</v>
+      <c r="A126" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="B127" s="15" t="s">
-        <v>257</v>
+      <c r="A127" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="B128" s="15" t="s">
-        <v>259</v>
+      <c r="A128" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="B129" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>262</v>
+      <c r="A129" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>268</v>
+        <v>74</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>269</v>
+        <v>77</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>270</v>
+        <v>212</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>271</v>
+        <v>78</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>272</v>
+        <v>213</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>276</v>
+        <v>79</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>278</v>
+        <v>81</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>280</v>
+        <v>218</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>282</v>
+        <v>82</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>294</v>
+        <v>83</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>295</v>
+        <v>228</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>300</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A149" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>302</v>
+      <c r="A151" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>304</v>
+      <c r="A152" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B152" s="15" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -2671,6 +2673,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B154">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3532,8 +3537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E15306-1EC0-7149-BCA9-9E710C9AE138}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>